<commit_message>
mapping borden + register
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bord" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Verkeersbordopstelling" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Verkeersteken" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="WegcodeRegister" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="555">
   <si>
     <t xml:space="preserve">Retroreflecterend verkeersbord</t>
   </si>
@@ -464,9 +466,6 @@
     <t xml:space="preserve">opstelling.wegsegmentid</t>
   </si>
   <si>
-    <t xml:space="preserve">niet ok, wegenregistersegment id’s zijn geen uri’s</t>
-  </si>
-  <si>
     <t xml:space="preserve">bron sqlite</t>
   </si>
   <si>
@@ -558,6 +557,1137 @@
   </si>
   <si>
     <t xml:space="preserve">gekozenBeheerder_fk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variabelOpschrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/bc70e37037baf3168de5e8942e4046de03fbddb3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1a. Gevaarlijke bocht. Bocht naar links.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/4c9ed6d1d0d5fd6d21213918b2091fa1fa8ec1a6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1b. Gevaarlijke bocht. Bocht naar rechts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/e91cbb3373c455fbe833179ab6c5481f91844f73.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1c. Gevaarlijke bocht. Dubbele bocht of opeenvolging van meer dan twee bochten, de eerste naar links.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/983a97862c32131603617087a786e939658e55b0.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1d. Gevaarlijke bocht. Dubbele bocht of opeenvolging van meer dan twee bochten, de eerste naar rechts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6efd0d51990f91a9847ad38b25c08b57373de02f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A3. Gevaarlijke daling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/8ea55712e37c795ad14816dd5d7bf328f35b31be.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A5. Steile helling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/0d3a8ad48eabcb07b66fb98ee43114bc7ad9a6c9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7a. Rijbaanversmalling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/35d0e370a3a6d08aa6a6d9fec5aa6bb813082510.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7b. Rijbaanversmalling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2584315ef09bc4d9042700908d5278f07129aec8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A7c. Rijbaanversmalling.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ead8258863436cf7788e3d3eea13ced8d2bf9f08.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A9. Beweegbare brug.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c92fb353a3b2bad8606eaa7ba0955df05c77951b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A11. Uitweg op een kaai of een oever.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/4c7d660ebff0b960ab66faa89255d2d794ca49c4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A13. Uitholling overdwars of ezelsrug.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c02b4c410e8af994328702a86c16bf0ba48c7593.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A14. Verhoogde inrichting(en).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/81ac056a77d9c3278fa899efe131608adf828183.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A15. Glibberige rijbaan. Het onderbord van volgend model mag gebruikt worden om aan te duiden dat de weg glad kan zijn ten gevolge van ijzel of sneeuw.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/84a16a148b0705fda9d3d5ce5b503c8c2aef352a.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A17. Kiezelprojectie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b701a4457aac9dba5dad45997f63155de68e744b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A19. Vallende stenen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2f22c62a9e76f39f69c2f2fc63d0b3a762798952.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A21. Oversteekplaats voor voetgangers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5f76d4009b9659fab704cd7b3763e6ba57a4f2e0.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A23. Plaats waar speciaal veel kinderen komen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5da483555ed76c2abfbba59f3fed6741ba594405.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A25. Oversteekplaats voor fietsers en bestuurders van tweewielige bromfietsen of plaats waar die bestuurders van een fietspad op de rijbaan komen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/756d74c5e7f27789c0bce357a996cbad498adeb1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A27. Doortocht van groot wild.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b37806024f811e83deadb5c2fb2e8a33c467df33.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A29. Doortocht van vee.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9204b2a513c3dec2f8a993f2721ad22ae1aeb227.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A31. Werken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/bdf77644f01cca1b2c8bb1f8c0eeda6cc4a0587a.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A33. Verkeerslichten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d518e401c1e97eae11384bb9b320eb7aca22ae30.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A35. Overtocht van vliegtuigen op geringe hoogte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/62fa21b1c4cc53bddfc7af884b9b1e2be0db3c50.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A37. Zijwind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9257f6e0a74a310903cfe12e444dcf36afe29a4c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A39. Verkeer toegelaten in twee richtingen na een gedeelte van de rijbaan met eenrichtingsverkeer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/3307f97d46f3244b0009cc206e34ab57e68819ea.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A41. Overweg met slagbomen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2a357279e336a43a8dc8582a653ff9af07b37fed.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A43. Overweg zonder slagbomen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/35a31d34223bbcda0075b959557da9723595b448.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A45. Overweg voor enkel spoor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c9dac5f5c385f741d813ef42a56063f3f70bbb86.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A47. Overweg voor twee of meer sporen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/70c830e55d23049014638322f39a794bc3086a53.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A49. Kruising van een openbare weg door een of meer in de rijbaan aangelegde sporen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/66435927bf28fa4d228cb32eef35c0395e7f3a07.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A50. File.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/8c1eee93f7065fc2f0872479b2c1dbeb077de9dc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A51. Gevaar dat niet door een speciaal symbool wordt bepaald. Een onderbord duidt de aard van het gevaar aan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b393ddf79c421f6ac49281e8eda589d7d5449ced.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B1. Voorrang verlenen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/93902196a98cd4a8150e589d3ebcb429b799fcb5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3. Verkeersbord dat het verkeersbord B1 aankondigt op de bij benadering aangeduide afstand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f9ccf0862e268c3bfaf5943027cbf3e90cf00cc3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5. Stoppen en voorrang verlenen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/1acf46db67fa271926bc387abc131ba315830946.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B7. Verkeersbord dat het verkeersbord B5 aankondigt op de bij benadering aangeduide afstand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/67a4dd01f9d061728d453c6be8e6f28854489cfd.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B9. Voorrangsweg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/3b16c71111e351b0a6e08ad275a99c79541f8d8b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B11. Einde van voorrangsweg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/223d99db3a625dd35f418681f8f1564e5d85e6c2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B13. Verkeersbord dat het verkeersbord B11 aankondigt op de bij benadering aangeduide afstand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/92b5fc03a0fde4c459df590ee918066a6fcc4528.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B15. Voorrang. De horizontale streep van het symbool mag worden gewijzigd om duidelijker plaatsgesteldheid weer te geven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/cacd023a6ab85793d1e85cf0b08e13231547c6a7.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B17. Kruispunt waar de voorrang van rechts geldt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/0c01d9f17150007e86e67beee3e439d0ebeb29eb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B19. Smalle doorgang. Gebod voorrang te verlenen aan de bestuurders die uit de tegenovergestelde richting komen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ec7c90d8d36f7568bafe2ddc5f96aa1d2856350b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B21. Smalle doorgang. Voorrang ten opzichte van de bestuurders die uit de tegenovergestelde richting komen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/24604e16189c0430a35cac3a3ae1c76dd2e4c0a3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B22. Krachtens verkeersbord B22 mogen fietsers en bestuurders van speed pedelecs de in artikel 61 en 62ter bedoelde verkeerslichten voorbijrijden om rechts af te slaan, wanneer het verkeerslicht op rood of oranjegeel staat, op voorwaarde dat zij hierbij voorrang verlenen aan de andere weggebruikers die zich verplaatsen op de openbare weg of op de rijbaan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b593576997842fc66b9c070f83dcd34ccd1c1fbf.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B23. Krachtens verkeersbord B23 mogen fietsers en bestuurders van speed pedelecs de in artikel 61 en 62ter bedoelde verkeerslichten voorbijrijden om rechtdoor te rijden, wanneer het verkeerslicht op rood of oranjegeel staat, op voorwaarde dat zij hierbij voorrang verlenen aan de andere weggebruikers die zich verplaatsen op de openbare weg of op de rijbaan vanaf het rode of oranjegele licht.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c3228803f146a2f6c9f2a8c5641a40746a541c1c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1. Verboden richting voor iedere bestuurder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d0954de4659a90055906d3a08e37cccab10aadc6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3. Verboden toegang, in beide richtingen, voor iedere bestuurder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/e82fcbf5043703908a11eb20c99b77b15a7da142.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C5. Verboden toegang voor bestuurders van motorvoertuigen met meer dan twee wielen en van motorfietsen met zijspan. Wanneer het verkeersbord is aangevuld met de vermelding "Uitgezonderd 2+" of "3+" zijn de rijbaan of de rijstrook aldus gesignaleerd, slechts toegankelijk voor voertuigen met ten minste 2 of 3 inzittenden, naargelang van de vermelding, evenals voor de voertuigen van de geregelde openbare diensten voor gemeenschappelijk vervoer. De andere voertuigen mogen de aldus gesignaleerde rijstroken slechts volgen: - om de op en afritten te gebruiken; - om van richting te veranderen of om een aanpalende eigendom te bereiken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f1052b169f8b01791d305233149dc0a2b28b8512.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6. Verboden toegang voor bestuurders van motorvoertuigen met vier wielen, geconstrueerd voor onverhard terrein, met een open carrosserie, een stuur als op een motorfiets en een zadel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f1c31ee557a39ff78566eb54e87e6dba710035ac.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7. Verboden toegang voor bestuurders van motorfietsen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/016723b4c3efd693021af4ee3c44e173de9a9b47.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9. Verboden toegang voor bestuurders van bromfietsen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d35502c87a3c50a7ebc04e79187b99dddbafff1b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11. Verboden toegang voor bestuurders van rijwielen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/52c914149e1e239404e68d723655c6f1c6fb0d8b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13. Verboden toegang voor bestuurders van gespannen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/0fb7c507f5a6f6635229975411064955c1d4b588.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C15. Verboden toegang voor ruiters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6e855fd92fefc38c9a5049b454d1ce1873ffe6c8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17. Verboden toegang voor bestuurders van handkarren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b47bd9473e41795e6b4580acc10539c10fb3cdca.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19. Verboden toegang voor voetgangers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/4b578a9d0554e876f7adaa06ce08fda0277bda8f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21. Verboden toegang voor bestuurders van voertuigen waarvan de massa in beladen toestand hoger is dan de aangeduide massa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/fb373f326dd12a1c29c291b5c93887701d0fa9f3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22. Verboden toegang voor bestuurders van autocars.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/302e2c22c0f59590cbe03bf6c399c593023af336.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23. Verboden toegang voor bestuurders van motorvoertuigen en slepen ontworpen en gebouwd voor het vervoer van goederen. Een opschrift op een onderbord beperkt het verbod tot de bestuurders van voertuigen of slepen waarvan de maximaal toegelaten massa hoger is dan de aangeduide massa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f6f5095a9ecc5ce0734c575669157e3a1f6e9a7d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24a. Verboden toegang voor bestuurders van voertuigen die de gevaarlijke goederen, bepaald door de voor vervoer van gevaarlijke goederen bevoegde Ministers, vervoeren. Een onderbord met vermelding van de letter B, C, D of E duidt aan dat het verbod geldt voor alle voertuigen die gevaarlijke goederen vervoeren waarvoor de toegang tot wegtunnels van respectievelijk categorie B, C, D of E verboden is, zoals deze categorieën voorzien zijn in &lt;a href="#art-1.9.5.2"&gt;artikel 1.9.5.2&lt;/a&gt; van bijlage A van het Europees verdrag betreffende het internationaal vervoer van gevaarlijke goederen over de weg (ADR), ondertekend te Genève op 30 september 1957.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/7520306498b5832a7b86d869dec335fc2189d6af.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24b. Verboden toegang voor bestuurders van voertuigen die de gevaarlijke ontvlambare of ontplofbare stoffen, bepaald door de voor vervoer van gevaarlijke goederen bevoegde Ministers, vervoeren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a3245c6b0d5cadd839a5659bf61a7fb437d142b1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24c. Verboden toegang voor bestuurders van voertuigen die de gevaarlijke verontreinigende stoffen, bepaald door de voor vervoer van gevaarlijke goederen bevoegde Ministers, vervoeren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/3dd4d828cd5248fbe1642f9418f6cf127d0c59a0.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25. Verboden toegang voor bestuurders van voertuigen of slepen waarvan de lengte, lading inbegrepen, groter is dan de aangeduide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/38080f54f78c64148108481d8c7de6edff8ddc4f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27. Verboden toegang voor bestuurders van voertuigen waarvan de breedte, lading inbegrepen, groter is dan de aangeduide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b705b3547eac782bed3f4464f1659aa48ac4682d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29. Verboden toegang voor bestuurders van voertuigen waarvan de hoogte, lading inbegrepen, groter is dan de aangeduide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9c71cc2c82e70830916be19487b5590233d47d4a.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31a. Verbod aan het volgend kruispunt af te slaan in de richting door de pijl aangegeven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9bb20517515bba06fdd10c7f851770c91208d227.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31b. Verbod aan het volgend kruispunt af te slaan in de richting door de pijl aangegeven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/81d3485ada845bca200a448783bd2f59d6f4104f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33. Vanaf het verkeersbord tot en met het volgend kruispunt, verbod te keren.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/028cea05d2e408948b9ce30221531a233ef8c33d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C35. Vanaf het verkeersbord tot en met het volgend kruispunt, verbod een gespan of een voertuig met meer dan twee wielen, links in te halen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6a4c17d53c46289a901a93378d43b1aaa53b70ad.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C37. Einde van het verbod opgelegd door het verkeersbord C35.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/19d926bd8cce096a3b1f1c1bbb838b38c09ba3be.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C39. Vanaf het verkeersbord tot en met het volgend kruispunt, verbod voor bestuurders van voertuigen of slepen gebruikt voor het vervoer van zaken, waarvan de maximale toegelaten massa meer dan 3.500 kg bedraagt, een gespan of een voertuig met meer dan twee wielen links in te halen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9c4cb2d285bbc58fea634454998bcd232b8cc399.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C41. Einde van het verbod opgelegd door het verkeersbord C39.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6e22b3782e9ab1b777deb72d8ea38fb370d8fd32.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C43. Vanaf het verkeersbord tot en met het volgend kruispunt, of tot elk verkeersbord C43 met of zonder zonale geldigheid, of tot het verkeersbord dat het begin of het einde van een bebouwde kom, van een woonerf of erf, of van een voetgangerszone aanduidt, verbod te rijden met een grotere snelheid dan deze die is aangeduid. - De vermelding "km" op het verkeersbord is facultatief. - Wanneer op een onderbord een bepaalde massa is aangeduid, is het verbod slechts van toepassing op voertuigen waarvan de maximale toegelaten massa hoger is dan de aangeduide. Het verkeersbord C43 met de vermelding 30 km per uur, geplaatst boven het verkeersbord F1, F1a of F1b is van toepassing op alle openbare wegen binnen de bebouwde kom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5c23dc8087f5b43bf7d60eef73d90ca055f1872c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C45. Einde van de snelheidsbeperking opgelegd door het verkeersbord C43. De vermelding "km" op het verkeersbord C45 is facultatief. Indien gebruik is gemaakt van het verkeersbord C43 met de vermelding 30 km per uur, geplaatst boven het verkeersbord F1, F1a of F1b, moet het verkeersbord C45 met dezelfde vermelding aangebracht zijn boven het verkeersbord F3, F3a of F3b van deze bebouwde kom.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ae9326d2bfcb937c6b331a9d51bf4ea55bfd7918.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C46. Einde van alle plaatselijke verbodsbepalingen opgelegd aan de voertuigen in beweging.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/bca5292cbc6c75945a9e742ca7759ade5edbf212.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C47. Tolpost. Verbod voorbij te rijden zonder te stoppen. Het opschrift mag vervangen worden door het woord "Taks".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/36ff976575ed7ab99391f6b97e2b72a882e14a0f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1. Verplichting de door de pijl aangeduide richting te volgen. De plaatsgesteldheid bepaalt de stand van de pijl. Wanneer het verkeersbord dat een niet-gebogen pijl voorstelt, op een hindernis geplaatst is, betekent het dat langs de door de pijl aangeduide richting moet voorbijgereden worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a1553a2c3dbbe50bbb4b69169c839aa7783e3fe6.png"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D1b. Verplichting de door de pijl aangeduide richting te volgen. De plaatsgesteldheid bepaalt de stand van de pijl. Wanneer het verkeersbord dat een niet-gebogen pijl voorstelt, op een hindernis geplaatst is, betekent het dat langs de door de pijl aangeduide richting moet voorbijgereden worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b83f3fdac64c3f24fd12382bd82ec48bc8d8449c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3. Verplichting één van de door de pijlen aangeduide richtingen te volgen. De plaatsgesteldheid bepaalt de stand van de pijlen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2366462c2d15bb44dd6e2fd61dca8c7bec2f31f5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D4. Verplichting voor voertuigen die gevaarlijke goederen vervoeren om de door de pijl aangeduide richting te volgen. De plaatsgesteldheid bepaalt de stand van de pijl. Een onderbord met vermelding van de letter B, C, D of E duidt erop dat de verplichting geldt voor voertuigen die gevaarlijke goederen vervoeren en waarvoor de toegang tot wegtunnels van respectievelijk categorie B, C, D of E verboden is, zoals deze categorieën voorzien zijn in &lt;a href="#art-1.9.5.2"&gt;artikel 1.9.5.2&lt;/a&gt; van bijlage A van het Europees verdrag betreffende het internationaal vervoer van gevaarlijke goederen over de weg (ADR.), ondertekend te Genève op 30 september 1957.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/00f7c93ae6ec2c0f97f2a66865f74e856f00b9ae.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5. Verplicht rondgaand verkeer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/08ba1399aaa37805a8f6d2d82c752ecde230ddb8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D7. Verplicht fietspad.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6502021f90d65b00c333568491c0c2758cf10c26.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D9. Deel van de openbare weg voorbehouden voor het verkeer van voetgangers, van fietsen en van tweewielige bromfietsen klasse A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/50584b9d14b21906c25c2b49683e7f80526d33c0.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10. Deel van de openbare weg voorbehouden voor het verkeer van voetgangers en fietsers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5362b3e4f97c8b963f61e8f55741b06c07add042.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D11. Verplichte weg voor voetgangers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2d5beaa4a4092dd7e83fe1f57a8acbcd29d2f2f2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D13. Verplichte weg voor ruiters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/4fa33a9e0ba10934059fc2345fa5935225b8dbc6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9a. Parkeren toegelaten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/8b198a670812348d341cede5272ce8e303f7534d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9b. Parkeren uitsluitend voor motorfietsen, personenauto's, auto's voor dubbelgebruik en minibussen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/3dbdf21ffd887a6576905ad20b28dff8560224dc.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9c. Parkeren uitsluitend voor lichte vrachtauto’s en vrachtauto’s.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c4f50bde4b8d867c88d88f9170c10d49342f73e5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9d. Parkeren uitsluitend voor autocars.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d948dee13da4c47543fac0edba48de4c69d6f551.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9e. Verplicht parkeren op de berm of op het trottoir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/627982af199988f31060045a751b887a309aef3a.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9f. Verplicht parkeren deels op de berm of op het trottoir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f8bec33bf361aec5f3a923d3f713301825f0d774.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9g. Verplicht parkeren op de rijbaan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c2c12f6a3c1a92f10d8fc11530efc1761458ed81.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9h. Parkeren uitsluitend voor kampeerauto's.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/244368a1d61b86e16eb0753dfe30b690b989ae5a.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9i. Parkeren uitsluitend voor motorfietsen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/1de938efbd840328afdd8753a9753a0ad560da38.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E9j. Parkeren voorbehouden voor fietsen van 7u30 tot 18u00 en voor motorfietsen, personenauto’s, auto’s voor dubbel gebruik en minibussen van 18u00 tot 7u30. Een opschrift of een symbool voorzien in artikel 70.2.1, 3° en 72.6, duidt de categorie van voertuigen of de specifieke parkeerregeling aan. Een opschrift duidt de tijdspanne van het voorbehouden parkeren of van de specifieke parkeerregeling aan. Het opschrift of het symbool mag ook op een onderbord worden afgebeeld.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5b8f964abf53d83a4f84b64ae02e81bfd62015e9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1a. Begin van een bebouwde kom. (Vlaams Gewest en Waals Gewest) Dit verkeersbord wordt rechts geplaatst op elke toegangsweg tot een bebouwde kom; het mag links herhaald worden. Wanneer binnen een bebouwde kom een verkeersbord C43 een andere snelheid aanduidt, dan geldt vanaf het volgend kruispunt opnieuw de maximumsnelheid van 50 km/u; Wanneer binnen een bebouwde kom een snelheidszone, een erf of een schoolomgeving wordt afgebakend, dan geldt vanaf het einde van de snelheidszone, het erf of de schoolomgeving opnieuw de maximumsnelheid van 50 km/u.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f41ff31f419f422c87e68e1f8a11af96b0e29e89.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1b. Begin van een bebouwde kom. (Vlaams Gewest en Waals Gewest) Dit verkeersbord wordt rechts geplaatst op elke toegangsweg tot een bebouwde kom; het mag links herhaald worden. Wanneer binnen een bebouwde kom een verkeersbord C43 een andere snelheid aanduidt, dan geldt vanaf het volgend kruispunt opnieuw de maximumsnelheid van 50 km/u; Wanneer binnen een bebouwde kom een snelheidszone, een erf of een schoolomgeving wordt afgebakend, dan geldt vanaf het einde van de snelheidszone, het erf of de schoolomgeving opnieuw de maximumsnelheid van 50 km/u.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/217552374d9a5b7f7cc1230f50a35e101c0bdee6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3a. Einde van een bebouwde kom. Dit verkeersbord wordt rechts geplaatst op elke uitvalsweg van een bebouwde kom; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/25aa0a1779d4e08f62248d3d5fdabcd144384ecd.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F3b. Einde van een bebouwde kom. Dit verkeersbord wordt rechts geplaatst op elke uitvalsweg van een bebouwde kom; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c5e17f6b95f150e9580d468e2d218a114fe8f61e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F4a. Begin van een zone met een snelheidsbeperking van 30 km per uur. Dit verkeersbord wordt rechts geplaatst aan elke toegang tot een zone met een snelheidsbeperking van 30 km per uur; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d060d7a1fea86221849be5fcdda717cd7889f876.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F4b. Einde van een zone met een snelheidsbeperking van 30 km per uur. Dit verkeersbord wordt rechts geplaatst aan elke uitgang van een zone met een snelheidsbeperking van 30 km per uur; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/bfb620a66014585886a3e1e788da8edc5a078784.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F5. Begin of oprit van een autosnelweg. De bijzondere verkeersregelen op de autosnelwegen gelden vanaf de plaats waar het verkeersbord aangebracht is. Dit verkeersbord wordt rechts geplaatst en mag links herhaald worden. Dit verkeersbord mag afgebeeld worden op de verkeersborden F25, F27, F29, F31, F39 en F41 om aan te duiden dat de gesignaleerde reisweg over een autosnelweg gaat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c64a22a33f69c5255ea356ac2687bdd190e92748.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F7. Einde van een autosnelweg. Dit verkeersbord wordt rechts geplaatst en mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2aac6272b0aeb16b26b8683957b0d968058d7351.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F8. Tunnel. Tunnel met een lengte van meer dan 500 meter. Op onderborden wordt de lengte van de tunnel en eventueel zijn naam aangeduid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/03d183a309d5c820067bcb8ead54392be6314dd7.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F9. Autoweg. De bijzondere verkeersregelen op de autowegen gelden vanaf de plaats waar het verkeersbord is aangebracht. Dit verkeersbord wordt rechts geplaatst en mag links herhaald worden. Dit verkeersbord mag afgebeeld worden op de verkeersborden F25, F27, F29, F31, F39 en F41 om aan te duiden dat de gesignaleerde reisweg over een autoweg gaat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ea909966fdb0cd38a6407ab366f11ee5c484e6be.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F11. Einde van een autoweg. Dit verkeersbord wordt rechts geplaatst en mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/2e642ae51c3fbc4b0adc54c012013014e236cecb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F12a. Begin van een woonerf of van een erf. De bijzondere verkeersregelen in de woonerven of erven gelden vanaf de plaats waar het verkeersbord aangebracht is. Dit verkeersbord wordt rechts geplaatst aan elke toegang tot een woonerf of erf; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/820e7161734bf5b2be2dcfa0391068dbe1c3ce95.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F12b. Einde van een woonerf of van een erf. Dit verkeersbord wordt rechts geplaatst aan elke uitgang van een woonerf of erf; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9c1752b655d18becf962d3de3feb6d952d1009ea.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F13. Verkeersbord dat pijlen op de rijbaan aankondigt en de keuze van een rijstrook voorschrijft. Dit verkeersbord kan de verschillende richtingen aanduiden. De streep tussen de rijstroken kan eventueel onderbroken zijn. Het bord mag aangevuld worden om de voorsorteringsstroken voorbehouden voor het verkeer van fietsers en bestuurders van tweewielige bromfietsen aan te duiden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f651e6989b1cf123fe7a5149fee186a54b8d7a67.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F14. Opstelvak voor fietsers en bestuurders van tweewielige bromfietsen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/1c2400698c0e5d3ec8e199af7c19673441311d4d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F15. Verkeersbord dat de keuze van een richting voorschrijft. - neerwaarts of opwaarts gerichte pijlen hebben betrekking op doorgaande richtingen; - schuin opwaarts of neerwaarts gerichte pijlen hebben betrekking op afslaande richtingen; - het aantal pijlen vertegenwoordigt het aantal rijstroken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/7189b2c0a35729e9596f9c9f7f3e884500bab2d3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F17. Aanduiding van de rijstroken van een rijbaan met een strook voorbehouden voor autobussen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/7050d8486c1a33afc3ec40611ed57bf52c2d6fd0.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F18. Aanwijzing van een bijzondere overrijdbare bedding, voorbehouden aan het verkeer van voertuigen van geregelde diensten voor gemeenschappelijk vervoer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5699d9d46c939f526876c7ced7ad7f7ff6ab71fe.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F19. Openbare weg met eenrichtingsverkeer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c5427810b51832ce573a2a482ed63e3b3d747b32.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F21. Rechts of links voorbijrijden toegelaten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d75963227e2f2e06d4b39bf0e040209f70fca85d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F23a. Nummer van een gewone weg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d8b4508af8df7279dfa1c0116867a4100678e9d9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F23b. Nummer van een autosnelweg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a9f21a130609d93ed5d58958484cf80f392eefca.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F23c. Nummer van een internationale weg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/78baf69f39d50b5a43b2693bd56340d54d3c4e22.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F23d. Nummer van een ring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/daad795898df12145b5500f98f4dfd3d2493cf70.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F25. Voorwegwijzer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/625f5862f204a885b5ee870578581331513bebb9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F27. Voorwegwijzer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c987017fac657ee7d2cab313dca47e35ab9c4a7d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F29. Wegwijzer. De afstand in km kan op de wegwijzer aangeduid zijn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/0933e3bf78fd67dde7f8883d06ed69066ddb20d9.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F31. Wegwijzer. Reisweg over een autosnelweg. De afstand in km kan op de wegwijzer aangeduid zijn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/45067baaa527c78033849ddfdc74fadd191deaf2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F33a. Bewegwijzeringsbord op afstand: luchthaven, universitair centrum, kliniek en ziekenhuis, beurs- of tentoonstellingshal, haven, wijk, ring, bedrijf, industriepark en commercieel centrum. De afstand in km kan op de wegwijzer aangeduid zijn. Het verkeersbord mag aangevuld worden met het symbool van het verkeersbord F53.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/67bb2e0452ac9d0781883a2fb923c61ccbc5e709.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F33b. Bewegwijzeringsbord op afstand: vallei of waterloop van toeristische aard. De afstand in km kan op de wegwijzer aangeduid zijn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ddb92e18feb889f999fdaa1c70f52bd6df9c4573.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F33c. Bewegwijzeringsbord op afstand: sportcentrum, plaats met een toeristisch of ontspannend karakter, recreatie- of pretpark, cultureel park, monument, merkwaardig landschap. Het verkeersbord mag aangevuld worden met de symbolen van het type S. 30. tot S. 36.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/31d9773144b1c9599235f2c7ea3dffbeb6d02c92.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F34a. Bewegwijzeringsbord in de nabijheid van inrichtingen en etablissementen die openbaar zijn of van algemeen belang, en in 't bijzonder: luchthaven, bibliotheek, post- en telefoonkantoor, brandweer en civiele bescherming, cultureel centrum of complex, animatiecentrum, openbaar centrum voor maatschappelijk welzijn (O.C.M.W.), begraafplaats, kliniek en ziekenhuis, politiediensten, onderwijsinstelling, station van de diensten voor het gemeenschappelijk vervoer, televisieomroep, plaats voor eredienst, museum, gerechtsgebouw, parking, haven, hulppost, taxatiekantoor, schouwburg, bedrijf, industriepark en commercieel centrum. Het verkeersbord mag aangevuld worden met het symbool van de verkeersborden F33a, F53, F55, F59 en F61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/feb5c87504de38b73f438fb85e522568fdb5130b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F34b.1. Wegwijzer: aanbevolen reisweg voor bepaalde categorieën van weggebruikers. Het verkeersbord wordt aangevuld met het (de) symbool(olen) van de verkeersborden C11, C15 en C19. De afstand in km en fracties van km kan op de wegwijzer aangeduid zijn. Op het verkeersbord F34b.2, zijn de vermelding van de bestemming en de pijl facultatief.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a0c2039a3291c5d563c87efb986f64f3bc228d05.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F34b.2. Wegwijzer: aanbevolen reisweg voor bepaalde categorieën van weggebruikers. Het verkeersbord wordt aangevuld met het (de) symbool(olen) van de verkeersborden C11, C15 en C19. De afstand in km en fracties van km kan op de wegwijzer aangeduid zijn. Op het verkeersbord F34b.2, zijn de vermelding van de bestemming en de pijl facultatief.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/85337d7fb64fdb5dd202d49d4ff39b93072866f1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F34c.1. Wegwijzer: aanbevolen reisweg naar een toeristische bestemming voor bepaalde categorieën van weggebruikers. Het verkeersbord wordt aangevuld met het (de) symbool(olen) van de verkeersborden C11, C15 en C19. De afstand in km en gedeelten van km kan op de wegwijzer aangeduid zijn. Op het verkeersbord F34c2, zijn de vermelding van de bestemming en de pijl facultatief.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/7b86dc0e348d9f5c2923856b5a97f057b2afc25e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F34c.2. Wegwijzer: aanbevolen reisweg naar een toeristische bestemming voor bepaalde categorieën van weggebruikers. Het verkeersbord wordt aangevuld met het (de) symbool(olen) van de verkeersborden C11, C15 en C19. De afstand in km en gedeelten van km kan op de wegwijzer aangeduid zijn. Op het verkeersbord F34c2, zijn de vermelding van de bestemming en de pijl facultatief.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6a816cc99e81759f4bbf8c2d33fad588c4776c04.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F35. Wegwijzer: sportcentrum, plaats met een toeristisch of ontspannend karakter, recreatie- of pretpark, cultureel park, monument, merkwaardig landschap, vereniging tot bevordering van het vreemdelingenverkeer. Het verkeersbord mag aangevuld worden met het symbool van het verkeersbord F77.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/12e965165a21f5dec12b62b33ec8a0804b3f5812.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F37. Wegwijzer: jeugdherberg, overnachtingsgelegenheden, kampeer- en caravanterrein, restaurant en vakantiedorp. Het verkeersbord mag aangevuld worden met de symbolen van de verkeersborden F65, F67, F71, F73 en F75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/e48bbdd53c1e2d6734c257990938958eb2d6a993.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F39. Voorwegwijzer die een omlegging aankondigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b14665e056d890ed16af2923136e878d6b5a510b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F41. Wegwijzer, omleggingsweg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/4e60bc25bb0cdc1ab397ec359ed06c39eba13dea.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F43. Plaatsnaambord.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9908211afd3e1afff3f4159e4564aeb807c56c30.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F45. Doodlopende weg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/eb5d9b052304404e6a817167c8a56acbb3e2225f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F45b. Doodlopende weg, uitgezonderd voor voetgangers en fietsers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/6d77f87bbcbb6e98ca5bdc68e45e7063a80c9a97.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F47. Einde van de werken.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/85b9432cb4fe31c2136d6762698490675f99f25f.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F49. Oversteekplaats voor voetgangers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/8b71ba495f02e99d9e499343afe3ab8016c241b8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F50. Oversteekplaats voor fietsers en bestuurders van tweewielige bromfietsen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f097a335ed5393e80e8118d47fc8314c5afcd0d8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F50bis. Verkeersbord dat de bestuurders die van richting veranderen wijst op fietsers en bestuurders van tweewielige bromfietsen die dezelfde openbare weg volgen. De reproduktie van het verkeersbord A25 kan vervangen worden door de reproduktie van het verkeersbord A21 om op een oversteekplaats voor voetgangers te wijzen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9b677011308ca505f600ed9020372980ac21b35b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F51. Ondergrondse of bovengrondse oversteekplaats voor voetgangers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/457d6826b66db799132a1513ac20eb253bf0a056.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F52. Aankondiging van een nooduitgang in tunnels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/8b1dc8d63d83d8de257eee01f80f86e9a8c798e5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F52bis. Vluchtroute. Aankondiging van de dichtstbijzijnde nooduitgang, in de aangeduide richting, in tunnels. De afstand in meter is aangeduid op het verkeersbord.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/90af760dff3755c44135b6faba685449edf3524e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F53. Verplegingsinrichting.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b413f7c1a5e5069146a7e820575ea4570f73b80d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F55. Hulppost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/26d6c81407ad549337bf7e26c1a6b752feaacb9b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F56. Brandblusapparaat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a41517f563571e05dc3056309328b2b38f84e600.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F57. Waterloop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/e7373f2e411d9b30ace9fd922ab8ef9a2899e22b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F59. Aankondiging van een parking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d5437cff41dcfd5b97bdc19a8f9b2a08cc6d61b3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F60. Aankondiging van een overdekte parking.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f727cdfe5df7c81fc66fe41b988fd61e3b3d4478.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F61. Telefoon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/253a8ef5a27191ca007e0cdea5a722ef8240bf11.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F62. Noodtelefoon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ee83980f782827a727e4cb4b3483be0f96627a0b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F63. Tankstation. Respectievelijk, van links naar rechts, benzine en diesel, LPG, CNG, LNG, H2, elektriciteit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/74d9071e82f5f901ac32ded7922063210e4b532e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F65. Hotel of motel.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b609ad01c8af6dd83da349d2348a6a143f27aeba.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F67. Restaurant.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a1664dc97d061fd83dfb9759d8905aa3866532fa.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F69. Drankgelegenheid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/56a77a2fe3da4b0a73ef5c7965076cbd7930a9db.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F71. Kampeerterrein.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/7287641403f42d6c7d5fe92b69166a7445ee8773.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F73. Caravanterrein.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/5eca2005cc0a4f5eba43eef1a26730b00f25cae0.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F75. Jeugdherberg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/7b9cc1a290df310c7d726dbdf08cc952ea150c32.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F77. Vereniging tot bevordering van het vreemdelingenverkeer, trefpunt voor toeristische informatie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/cfa6a9bb9d43cf9771102c77af4ca1f313b330f5.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F79. Voorwegwijzer die de vermindering van het aantal rijstroken aankondigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d78b183c0211400d4a7d0bfe89818246191eb6a8.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F81. Voorwegwijzer die een uitwijking aankondigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/4c485b4a8d41942f3234840d97cb889ae35d5391.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F83. Voorwegwijzer die een doorsteek van de middenberm aankondigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9898d8dde8a698ede1e1c11e2e1e0d8d7a00e479.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F85. Verkeer toegelaten in beide richtingen op een deel van de rijbaan met eenrichtingsverkeer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a88ac4c5d7a80fc9d7ec407d9af237202cb86ad4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F87. Verhoogde inrichting(en).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/3a40becef603e84f3a08e6b13db90378fc6d838d.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F89. Voorwegwijzer die een gevaar of een verkeersregel aankondigt die slechts van toepassing is op een of meerdere rijstroken van een rijbaan die meerdere rijstroken in dezelfde richting omvat. Dit verkeersbord mag niet boven de rijbaan geplaatst worden. De aankondiging van een gevaar of een verkeersregel kan boven de rijbaan aangebracht worden, boven de rijstrook waarvoor ze bestemd is, zonder dat het verkeersbord F89 geplaatst wordt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/bf8a808389e86d54abafbd03c9293c97a1e728d6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F91. Verkeersbord dat een gevaar aanduidt of een verkeersregel voorschrijft die slechts van toepassing is op één of meerdere rijstroken van een rijbaan die meerdere rijstroken in dezelfde richting omvat. Dit verkeersbord mag niet boven de rijbaan geplaatst worden. De aankondiging van een gevaar of een verkeersregel kan boven de rijbaan aangebracht worden, boven de rijstrook waarvoor ze bestemd is, zonder dat het verkeersbord F91 geplaatst wordt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/41fb15170c03a7c4cc1f94a42cc21c58f313db83.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F93. Verkeersbord dat een radio-omroep aanduidt waar verkeersinformatie gegeven wordt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a2153e51b314c9491a8259465949ac5df8949a92.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F95. Noodstopstrook. Het symbool mag aangepast worden om duidelijker de plaatsgesteldheid weer te geven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d6fef6aba9c22181d8d028eed5d7cb7516f711e4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F97. Verkeersbord dat een versmalling aanduidt die de omvang van een rijstrook heeft. Het symbool mag aangepast worden om duidelijker de plaatsgesteldheid weer te geven.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/50c660e6ba944c983d58f9996a8b28226c79fe28.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F98. Vluchthaven. Een onderbord met volgende symbolen duidt aan dat de vluchthaven uitgerust is met een noodtelefoon en een brandblusser.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/ae152c275bbb8adc8c3271668b0a4880dbfa7ac3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F99a. Weg of deel van de openbare weg voorbehouden voor het verkeer van voetgangers, fietsers, ruiters en bestuurders van speed pedelecs. Het verkeersbord mag aangepast worden volgens de categorie(ën) van weggebruiker(s) die tot deze weg is (zijn) toegelaten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/24abcc7e3c5c87a6a84bcb13a5719051c47ec8e7.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F99b. Weg of deel van de openbare weg voorbehouden voor het verkeer van voetgangers, fietsers, ruiters en bestuurders van speed pedelecs met aanduiding van het deel van de weg dat bestemd is voor de verschillende categorieën van weggebruikers. Het verkeersbord mag aangepast worden volgens de categorie(ën) van weggebruiker(s) die tot deze weg is (zijn) toegelaten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/8dc5cd1c92e2ab8e813ef0430702020aed8db741.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F99c. Weg voorbehouden voor landbouwvoertuigen, voetgangers, fietsers, ruiters en bestuurders van speed pedelecs. Het verkeersbord mag aangepast worden volgens de categorieën van weggebruikers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/3d2020796751e92ac8b3b6e1c457a9839f416fbf.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F101a. Einde van de weg of van het deel van de openbare weg voorbehouden voor het verkeer van voetgangers, fietsers, ruiters en bestuurders van speed pedelecs. Het verkeersbord mag aangepast worden volgens de categorie(ën) van weggebruiker(s) die tot deze weg is (zijn) toegelaten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/e3cf550f6abdda5a224e9bd83feeacb10c10cc1c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F101b. Einde van de weg of deel van de openbare weg voorbehouden voor het verkeer van voetgangers, fietsers, ruiters en bestuurders van speed pedelecs met aanduiding van het deel van de weg dat bestemd is voor de verschillende categorieën van weggebruikers. Het verkeersbord mag aangepast worden volgens de categorie(ën) van weggebruiker(s), die tot deze weg is (zijn) toegelaten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/9c0211493da44156892aaf836ac49a34e6a7ea8e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F101c. Einde van de weg voorbehouden voor landbouwvoertuigen, voetgangers, fietsers, ruiters en bestuurders van speed pedelecs. Het verkeersbord mag aangepast worden volgens de categorieën van weggebruikers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f0e73d8d3d19078e36e79cfb08bee72089f805a4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F103. Begin van een voetgangerszone. Dit verkeersbord wordt rechts geplaatst aan elke toegang tot een voetgangerszone; het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/b05e5dd4d95488053b9c603aea529525fb8bf2a6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F105. Einde van een voetgangerszone. Dit verkeersbord wordt rechts geplaatst aan elke uitgang van een voetgangerszone. Het mag links herhaald worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/886970a5d74416430ec3bcf4209235faed80e967.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F111. Fietsstraat.  De fietsstraat eindigt ter hoogte van het volgend kruispunt of ter hoogte van het verkeersbord F113. De vermelding ""Fietsstraat"" op het verkeersbord is facultatief."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/c221b43985b205dfd4e8e59226a48c9d6271c81c.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F113. Einde van een fietsstraat. De vermelding “Fietsstraat” op het verkeersbord is facultatief."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/a7c43434517d24851ae1e276f0f4ee522bd6ee4e.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F117. Begin van een lage emissiezone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/d412f98be686536778e92b5e4ca2fcfeb19ca3ca.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F118. Einde van een lage emissiezone.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/72a2609804a0d2f45716cc01955f33f6e8e2d4d4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F119. Begin van een luchthavengebied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/image/orig/f87777ad32c50db66ea161a7ac46d2aec71812c6.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F120. Einde van een luchthavengebied.</t>
   </si>
 </sst>
 </file>
@@ -567,7 +1697,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -603,8 +1733,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,12 +1756,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFBF00"/>
         <bgColor rgb="FFFF9900"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF4000"/>
-        <bgColor rgb="FFC9211E"/>
       </patternFill>
     </fill>
   </fills>
@@ -664,7 +1793,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -697,7 +1826,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -757,7 +1890,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF4000"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -780,11 +1913,11 @@
   </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.36"/>
@@ -1453,10 +2586,10 @@
   <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
@@ -1604,11 +2737,11 @@
         <v>145</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="I8" s="8" t="s">
-        <v>147</v>
+      <c r="I8" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +2879,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,7 +2889,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,7 +2899,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,32 +2909,32 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,17 +2944,17 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,17 +2964,17 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1861,7 +2994,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,83 +3004,1643 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B188"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B142" activeCellId="0" sqref="B142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="61.69"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>357</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>361</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>363</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>373</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>377</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>387</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>393</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>395</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>425</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="B176" s="9" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="B177" s="9" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="B179" s="9" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="B181" s="9" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>541</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>543</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>545</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="B187" s="0" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>553</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>